<commit_message>
Commit source change DB and processor
</commit_message>
<xml_diff>
--- a/Danh-sách-cp.xlsx
+++ b/Danh-sách-cp.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lana\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PhatHuy\Desktop\S\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -9215,7 +9215,7 @@
   <dimension ref="A1:D1476"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25598,7 +25598,6 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D1476"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>